<commit_message>
Error Fixed For DBNull Values in Rows
</commit_message>
<xml_diff>
--- a/Player_Data.xlsx
+++ b/Player_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\personal\GitHBIO\HBIO-DataServices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HBIO-DataServices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D73C02-D3BA-4B8A-88B2-9BB63C1A6CE6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30277572-1C53-488C-9F53-3DF1EA3520B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1887,13 +1887,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -1901,8 +1903,8 @@
     <col min="8" max="8" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="22.28515625" bestFit="1" customWidth="1"/>

</xml_diff>